<commit_message>
Time to Dead Pool - Add paleo events
A start for the plot. Comments list additional changes.
</commit_message>
<xml_diff>
--- a/TimeToDeadPool/DroughtDurations.xlsx
+++ b/TimeToDeadPool/DroughtDurations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverFutures\TimeToDeadPool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A9CAA30-A44E-42DB-9C21-14FBE24386DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09573EC-4FC0-4E00-B94D-10E6ED28BEA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6060" xr2:uid="{943A7962-CCF4-40C6-97E8-CAD00CAAC7B2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t>Colorado River Key Droughts</t>
   </si>
@@ -48,19 +48,10 @@
     <t>Meko et al 2017</t>
   </si>
   <si>
-    <t>Meko et al 2018</t>
-  </si>
-  <si>
     <t>Observed</t>
   </si>
   <si>
     <t>Woodhouse et al (2006)</t>
-  </si>
-  <si>
-    <t>Meko et al 2019</t>
-  </si>
-  <si>
-    <t>Meko et al 2020</t>
   </si>
   <si>
     <t>Pulled from Homa/Dave T dotty plots</t>
@@ -464,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{583A50FA-A299-4B97-8B43-95D012DE7FB6}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,7 +473,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -533,7 +524,7 @@
         <v>25</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -550,7 +541,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -567,7 +558,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -584,7 +575,7 @@
         <v>25</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -602,7 +593,7 @@
         <v>508</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -620,7 +611,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -638,7 +629,7 @@
         <v>4</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -656,7 +647,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -674,7 +665,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -692,7 +683,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -710,7 +701,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -728,7 +719,7 @@
         <v>3</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -746,7 +737,7 @@
         <v>600</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>